<commit_message>
Correção Royalties by Channell UBC
</commit_message>
<xml_diff>
--- a/data/mapping/mapping-rubricas.xlsx
+++ b/data/mapping/mapping-rubricas.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ROYALTY\_ANALYTICS_\Python Codes\Nas Nuvens App\nasnuvens-app\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ROYALTY\_ANALYTICS_\Python Codes\Nas Nuvens App\nasnuvens-app\data\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393132CA-BFE0-492E-99B5-79735F7C69F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC9AB58-0E08-4673-99D1-478E054DB12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$1034</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$1397</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2794" uniqueCount="1407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2798" uniqueCount="1409">
   <si>
     <t>SHOW</t>
   </si>
@@ -4257,6 +4257,12 @@
   </si>
   <si>
     <t>Channel</t>
+  </si>
+  <si>
+    <t>AP-ALTERNATIVO TV BAND</t>
+  </si>
+  <si>
+    <t>AP-REDE TV! + DG</t>
   </si>
 </sst>
 </file>
@@ -4321,47 +4327,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4670,10 +4636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1397"/>
+  <dimension ref="A1:B1399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1361" workbookViewId="0">
-      <selection activeCell="A1396" sqref="A1396"/>
+    <sheetView tabSelected="1" topLeftCell="A1363" workbookViewId="0">
+      <selection activeCell="B1399" sqref="B1399"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15858,11 +15824,29 @@
         <v>1036</v>
       </c>
     </row>
+    <row r="1398" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1398" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1398" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1399" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B1399" t="s">
+        <v>1034</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B1034" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B1397">
     <sortCondition ref="A2:A1397"/>
   </sortState>
+  <conditionalFormatting sqref="A2:A1397">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>